<commit_message>
Modified HVAC assembly information
Updated documentation accordingly
</commit_message>
<xml_diff>
--- a/cea/databases/DE/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/DE/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge38yoz\CityEnergyAnalyst\cea\databases\DE\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632C6074-1854-4CC6-871B-061D5B27C02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9867CCA-8B50-4D64-AE68-98268420F287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5168" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5168" uniqueCount="1239">
   <si>
     <t>STANDARD</t>
   </si>
@@ -3809,6 +3809,9 @@
   </si>
   <si>
     <t>WINDOW_HR-EAST_G_AR</t>
+  </si>
+  <si>
+    <t>HVAC_VENTILATION_AS0</t>
   </si>
 </sst>
 </file>
@@ -7726,12 +7729,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
       <selection activeCell="N2" sqref="N2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G152" sqref="G152"/>
+      <selection pane="bottomRight" activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19038,17 +19041,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J191"/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C119" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B109" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D11" sqref="D11"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G125" sqref="G125:J148"/>
+      <selection pane="bottomRight" activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="62" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="62" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="62" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" style="62" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" style="62" bestFit="1" customWidth="1"/>
@@ -19093,7 +19096,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="63" t="s">
         <v>742</v>
       </c>
@@ -19110,7 +19113,7 @@
         <v>723</v>
       </c>
       <c r="F2" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G2" s="120" t="s">
         <v>725</v>
@@ -19125,7 +19128,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="70" t="s">
         <v>743</v>
       </c>
@@ -19141,8 +19144,8 @@
       <c r="E3" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>724</v>
+      <c r="F3" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G3" s="120" t="s">
         <v>725</v>
@@ -19157,7 +19160,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="70" t="s">
         <v>744</v>
       </c>
@@ -19174,7 +19177,7 @@
         <v>723</v>
       </c>
       <c r="F4" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G4" s="120" t="s">
         <v>725</v>
@@ -19189,7 +19192,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="70" t="s">
         <v>745</v>
       </c>
@@ -19205,8 +19208,8 @@
       <c r="E5" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>724</v>
+      <c r="F5" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G5" s="120" t="s">
         <v>725</v>
@@ -19221,7 +19224,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="70" t="s">
         <v>746</v>
       </c>
@@ -19238,7 +19241,7 @@
         <v>723</v>
       </c>
       <c r="F6" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G6" s="120" t="s">
         <v>725</v>
@@ -19253,7 +19256,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="70" t="s">
         <v>747</v>
       </c>
@@ -19269,8 +19272,8 @@
       <c r="E7" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>724</v>
+      <c r="F7" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G7" s="120" t="s">
         <v>725</v>
@@ -19285,7 +19288,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="70" t="s">
         <v>748</v>
       </c>
@@ -19302,7 +19305,7 @@
         <v>723</v>
       </c>
       <c r="F8" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G8" s="120" t="s">
         <v>725</v>
@@ -19317,7 +19320,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="70" t="s">
         <v>749</v>
       </c>
@@ -19333,8 +19336,8 @@
       <c r="E9" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>724</v>
+      <c r="F9" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G9" s="120" t="s">
         <v>725</v>
@@ -19349,7 +19352,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="70" t="s">
         <v>750</v>
       </c>
@@ -19366,7 +19369,7 @@
         <v>723</v>
       </c>
       <c r="F10" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G10" s="120" t="s">
         <v>725</v>
@@ -19381,7 +19384,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="70" t="s">
         <v>751</v>
       </c>
@@ -19397,8 +19400,8 @@
       <c r="E11" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>724</v>
+      <c r="F11" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G11" s="120" t="s">
         <v>725</v>
@@ -19413,7 +19416,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="70" t="s">
         <v>752</v>
       </c>
@@ -19430,7 +19433,7 @@
         <v>723</v>
       </c>
       <c r="F12" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G12" s="120" t="s">
         <v>725</v>
@@ -19445,7 +19448,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="124" t="s">
         <v>753</v>
       </c>
@@ -19461,8 +19464,8 @@
       <c r="E13" s="126" t="s">
         <v>723</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>724</v>
+      <c r="F13" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G13" s="120" t="s">
         <v>725</v>
@@ -19477,7 +19480,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="76" t="s">
         <v>16</v>
       </c>
@@ -19494,7 +19497,7 @@
         <v>723</v>
       </c>
       <c r="F14" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G14" s="120" t="s">
         <v>725</v>
@@ -19509,7 +19512,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="78" t="s">
         <v>17</v>
       </c>
@@ -19525,8 +19528,8 @@
       <c r="E15" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>724</v>
+      <c r="F15" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G15" s="120" t="s">
         <v>725</v>
@@ -19541,7 +19544,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="78" t="s">
         <v>19</v>
       </c>
@@ -19558,7 +19561,7 @@
         <v>723</v>
       </c>
       <c r="F16" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G16" s="120" t="s">
         <v>725</v>
@@ -19573,7 +19576,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="78" t="s">
         <v>21</v>
       </c>
@@ -19589,8 +19592,8 @@
       <c r="E17" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>724</v>
+      <c r="F17" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G17" s="120" t="s">
         <v>725</v>
@@ -19605,7 +19608,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="78" t="s">
         <v>23</v>
       </c>
@@ -19622,7 +19625,7 @@
         <v>723</v>
       </c>
       <c r="F18" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G18" s="120" t="s">
         <v>725</v>
@@ -19637,7 +19640,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="78" t="s">
         <v>25</v>
       </c>
@@ -19653,8 +19656,8 @@
       <c r="E19" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>724</v>
+      <c r="F19" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G19" s="120" t="s">
         <v>725</v>
@@ -19669,7 +19672,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="78" t="s">
         <v>27</v>
       </c>
@@ -19686,7 +19689,7 @@
         <v>723</v>
       </c>
       <c r="F20" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G20" s="120" t="s">
         <v>725</v>
@@ -19701,7 +19704,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="78" t="s">
         <v>29</v>
       </c>
@@ -19717,8 +19720,8 @@
       <c r="E21" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>724</v>
+      <c r="F21" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G21" s="120" t="s">
         <v>725</v>
@@ -19733,7 +19736,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="78" t="s">
         <v>31</v>
       </c>
@@ -19750,7 +19753,7 @@
         <v>723</v>
       </c>
       <c r="F22" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G22" s="120" t="s">
         <v>725</v>
@@ -19765,7 +19768,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="78" t="s">
         <v>33</v>
       </c>
@@ -19781,8 +19784,8 @@
       <c r="E23" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>724</v>
+      <c r="F23" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G23" s="120" t="s">
         <v>725</v>
@@ -19797,7 +19800,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="78" t="s">
         <v>35</v>
       </c>
@@ -19814,7 +19817,7 @@
         <v>723</v>
       </c>
       <c r="F24" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G24" s="120" t="s">
         <v>725</v>
@@ -19829,7 +19832,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="79" t="s">
         <v>37</v>
       </c>
@@ -19845,8 +19848,8 @@
       <c r="E25" s="126" t="s">
         <v>723</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>724</v>
+      <c r="F25" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G25" s="120" t="s">
         <v>725</v>
@@ -19861,7 +19864,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="127" t="s">
         <v>39</v>
       </c>
@@ -19878,7 +19881,7 @@
         <v>723</v>
       </c>
       <c r="F26" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G26" s="120" t="s">
         <v>725</v>
@@ -19893,7 +19896,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="87" t="s">
         <v>41</v>
       </c>
@@ -19909,8 +19912,8 @@
       <c r="E27" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>724</v>
+      <c r="F27" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G27" s="120" t="s">
         <v>725</v>
@@ -19925,7 +19928,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="87" t="s">
         <v>43</v>
       </c>
@@ -19942,7 +19945,7 @@
         <v>723</v>
       </c>
       <c r="F28" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G28" s="120" t="s">
         <v>725</v>
@@ -19957,7 +19960,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="87" t="s">
         <v>45</v>
       </c>
@@ -19973,8 +19976,8 @@
       <c r="E29" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>724</v>
+      <c r="F29" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G29" s="120" t="s">
         <v>725</v>
@@ -19989,7 +19992,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="87" t="s">
         <v>47</v>
       </c>
@@ -20006,7 +20009,7 @@
         <v>723</v>
       </c>
       <c r="F30" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G30" s="120" t="s">
         <v>725</v>
@@ -20021,7 +20024,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="87" t="s">
         <v>49</v>
       </c>
@@ -20037,8 +20040,8 @@
       <c r="E31" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>724</v>
+      <c r="F31" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G31" s="120" t="s">
         <v>725</v>
@@ -20053,7 +20056,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="87" t="s">
         <v>51</v>
       </c>
@@ -20070,7 +20073,7 @@
         <v>723</v>
       </c>
       <c r="F32" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G32" s="120" t="s">
         <v>725</v>
@@ -20085,7 +20088,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="87" t="s">
         <v>53</v>
       </c>
@@ -20101,8 +20104,8 @@
       <c r="E33" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>724</v>
+      <c r="F33" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G33" s="120" t="s">
         <v>725</v>
@@ -20117,7 +20120,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="87" t="s">
         <v>55</v>
       </c>
@@ -20134,7 +20137,7 @@
         <v>723</v>
       </c>
       <c r="F34" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G34" s="120" t="s">
         <v>725</v>
@@ -20149,7 +20152,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="87" t="s">
         <v>57</v>
       </c>
@@ -20165,8 +20168,8 @@
       <c r="E35" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>724</v>
+      <c r="F35" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G35" s="120" t="s">
         <v>725</v>
@@ -20181,7 +20184,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="89" t="s">
         <v>59</v>
       </c>
@@ -20198,7 +20201,7 @@
         <v>723</v>
       </c>
       <c r="F36" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G36" s="120" t="s">
         <v>725</v>
@@ -20213,7 +20216,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="92" t="s">
         <v>61</v>
       </c>
@@ -20229,8 +20232,8 @@
       <c r="E37" s="121" t="s">
         <v>723</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>724</v>
+      <c r="F37" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G37" s="120" t="s">
         <v>725</v>
@@ -20245,7 +20248,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="94" t="s">
         <v>63</v>
       </c>
@@ -20262,7 +20265,7 @@
         <v>723</v>
       </c>
       <c r="F38" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G38" s="120" t="s">
         <v>725</v>
@@ -20277,7 +20280,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="94" t="s">
         <v>65</v>
       </c>
@@ -20293,8 +20296,8 @@
       <c r="E39" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F39" s="6" t="s">
-        <v>724</v>
+      <c r="F39" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G39" s="120" t="s">
         <v>725</v>
@@ -20309,7 +20312,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="94" t="s">
         <v>67</v>
       </c>
@@ -20326,7 +20329,7 @@
         <v>723</v>
       </c>
       <c r="F40" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G40" s="120" t="s">
         <v>725</v>
@@ -20341,7 +20344,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="95" t="s">
         <v>69</v>
       </c>
@@ -20357,8 +20360,8 @@
       <c r="E41" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>724</v>
+      <c r="F41" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G41" s="129" t="s">
         <v>725</v>
@@ -20373,7 +20376,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="99" t="s">
         <v>71</v>
       </c>
@@ -20389,8 +20392,8 @@
       <c r="E42" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>724</v>
+      <c r="F42" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G42" s="129" t="s">
         <v>725</v>
@@ -20405,7 +20408,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="99" t="s">
         <v>73</v>
       </c>
@@ -20421,8 +20424,8 @@
       <c r="E43" s="126" t="s">
         <v>723</v>
       </c>
-      <c r="F43" s="6" t="s">
-        <v>724</v>
+      <c r="F43" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G43" s="120" t="s">
         <v>725</v>
@@ -20437,12 +20440,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>754</v>
       </c>
-      <c r="B44" s="119" t="s">
-        <v>720</v>
+      <c r="B44" s="123" t="s">
+        <v>728</v>
       </c>
       <c r="C44" s="35" t="s">
         <v>721</v>
@@ -20453,8 +20456,8 @@
       <c r="E44" s="121" t="s">
         <v>723</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>724</v>
+      <c r="F44" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G44" s="132" t="s">
         <v>725</v>
@@ -20469,12 +20472,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>755</v>
       </c>
-      <c r="B45" s="123" t="s">
-        <v>720</v>
+      <c r="B45" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C45" s="39" t="s">
         <v>721</v>
@@ -20485,8 +20488,8 @@
       <c r="E45" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F45" s="6" t="s">
-        <v>724</v>
+      <c r="F45" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G45" s="120" t="s">
         <v>725</v>
@@ -20501,12 +20504,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>756</v>
       </c>
       <c r="B46" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C46" s="93" t="s">
         <v>721</v>
@@ -20518,7 +20521,7 @@
         <v>723</v>
       </c>
       <c r="F46" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G46" s="120" t="s">
         <v>725</v>
@@ -20533,12 +20536,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>757</v>
       </c>
-      <c r="B47" s="123" t="s">
-        <v>720</v>
+      <c r="B47" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C47" s="39" t="s">
         <v>721</v>
@@ -20549,8 +20552,8 @@
       <c r="E47" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F47" s="6" t="s">
-        <v>724</v>
+      <c r="F47" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G47" s="120" t="s">
         <v>725</v>
@@ -20565,12 +20568,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>758</v>
       </c>
       <c r="B48" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C48" s="93" t="s">
         <v>721</v>
@@ -20582,7 +20585,7 @@
         <v>723</v>
       </c>
       <c r="F48" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G48" s="120" t="s">
         <v>725</v>
@@ -20597,12 +20600,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>759</v>
       </c>
-      <c r="B49" s="123" t="s">
-        <v>720</v>
+      <c r="B49" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C49" s="39" t="s">
         <v>721</v>
@@ -20613,8 +20616,8 @@
       <c r="E49" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F49" s="6" t="s">
-        <v>724</v>
+      <c r="F49" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G49" s="120" t="s">
         <v>725</v>
@@ -20629,12 +20632,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>760</v>
       </c>
       <c r="B50" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C50" s="93" t="s">
         <v>721</v>
@@ -20646,7 +20649,7 @@
         <v>723</v>
       </c>
       <c r="F50" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G50" s="120" t="s">
         <v>725</v>
@@ -20661,11 +20664,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>761</v>
       </c>
-      <c r="B51" s="123" t="s">
+      <c r="B51" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C51" s="39" t="s">
@@ -20677,8 +20680,8 @@
       <c r="E51" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>724</v>
+      <c r="F51" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G51" s="120" t="s">
         <v>725</v>
@@ -20693,7 +20696,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>762</v>
       </c>
@@ -20710,7 +20713,7 @@
         <v>723</v>
       </c>
       <c r="F52" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G52" s="120" t="s">
         <v>725</v>
@@ -20725,11 +20728,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>763</v>
       </c>
-      <c r="B53" s="123" t="s">
+      <c r="B53" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C53" s="39" t="s">
@@ -20741,8 +20744,8 @@
       <c r="E53" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F53" s="6" t="s">
-        <v>724</v>
+      <c r="F53" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G53" s="120" t="s">
         <v>725</v>
@@ -20757,7 +20760,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>764</v>
       </c>
@@ -20774,7 +20777,7 @@
         <v>723</v>
       </c>
       <c r="F54" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G54" s="120" t="s">
         <v>725</v>
@@ -20789,7 +20792,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>765</v>
       </c>
@@ -20805,8 +20808,8 @@
       <c r="E55" s="126" t="s">
         <v>723</v>
       </c>
-      <c r="F55" s="6" t="s">
-        <v>724</v>
+      <c r="F55" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G55" s="120" t="s">
         <v>725</v>
@@ -20821,12 +20824,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B56" s="119" t="s">
-        <v>720</v>
+      <c r="B56" s="123" t="s">
+        <v>728</v>
       </c>
       <c r="C56" s="93" t="s">
         <v>721</v>
@@ -20838,7 +20841,7 @@
         <v>723</v>
       </c>
       <c r="F56" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G56" s="120" t="s">
         <v>725</v>
@@ -20853,12 +20856,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B57" s="123" t="s">
-        <v>720</v>
+      <c r="B57" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C57" s="39" t="s">
         <v>721</v>
@@ -20869,8 +20872,8 @@
       <c r="E57" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F57" s="6" t="s">
-        <v>724</v>
+      <c r="F57" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G57" s="120" t="s">
         <v>725</v>
@@ -20885,12 +20888,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="17" t="s">
         <v>91</v>
       </c>
       <c r="B58" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C58" s="93" t="s">
         <v>721</v>
@@ -20902,7 +20905,7 @@
         <v>723</v>
       </c>
       <c r="F58" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G58" s="120" t="s">
         <v>725</v>
@@ -20917,12 +20920,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B59" s="123" t="s">
-        <v>720</v>
+      <c r="B59" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C59" s="39" t="s">
         <v>721</v>
@@ -20933,8 +20936,8 @@
       <c r="E59" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F59" s="6" t="s">
-        <v>724</v>
+      <c r="F59" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G59" s="120" t="s">
         <v>725</v>
@@ -20949,12 +20952,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="17" t="s">
         <v>95</v>
       </c>
       <c r="B60" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C60" s="93" t="s">
         <v>721</v>
@@ -20966,7 +20969,7 @@
         <v>723</v>
       </c>
       <c r="F60" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G60" s="120" t="s">
         <v>725</v>
@@ -20981,12 +20984,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="123" t="s">
-        <v>720</v>
+      <c r="B61" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C61" s="39" t="s">
         <v>721</v>
@@ -20997,8 +21000,8 @@
       <c r="E61" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F61" s="6" t="s">
-        <v>724</v>
+      <c r="F61" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G61" s="120" t="s">
         <v>725</v>
@@ -21013,12 +21016,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
         <v>99</v>
       </c>
       <c r="B62" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C62" s="93" t="s">
         <v>721</v>
@@ -21030,7 +21033,7 @@
         <v>723</v>
       </c>
       <c r="F62" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G62" s="120" t="s">
         <v>725</v>
@@ -21045,11 +21048,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B63" s="123" t="s">
+      <c r="B63" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C63" s="39" t="s">
@@ -21061,8 +21064,8 @@
       <c r="E63" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F63" s="6" t="s">
-        <v>724</v>
+      <c r="F63" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G63" s="120" t="s">
         <v>725</v>
@@ -21077,7 +21080,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
         <v>103</v>
       </c>
@@ -21094,7 +21097,7 @@
         <v>723</v>
       </c>
       <c r="F64" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G64" s="120" t="s">
         <v>725</v>
@@ -21109,11 +21112,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B65" s="123" t="s">
+      <c r="B65" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C65" s="39" t="s">
@@ -21125,8 +21128,8 @@
       <c r="E65" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F65" s="6" t="s">
-        <v>724</v>
+      <c r="F65" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G65" s="120" t="s">
         <v>725</v>
@@ -21141,7 +21144,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
         <v>107</v>
       </c>
@@ -21158,7 +21161,7 @@
         <v>723</v>
       </c>
       <c r="F66" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G66" s="120" t="s">
         <v>725</v>
@@ -21173,7 +21176,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="21" t="s">
         <v>109</v>
       </c>
@@ -21189,8 +21192,8 @@
       <c r="E67" s="126" t="s">
         <v>723</v>
       </c>
-      <c r="F67" s="6" t="s">
-        <v>724</v>
+      <c r="F67" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G67" s="120" t="s">
         <v>725</v>
@@ -21205,12 +21208,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B68" s="119" t="s">
-        <v>720</v>
+      <c r="B68" s="123" t="s">
+        <v>728</v>
       </c>
       <c r="C68" s="93" t="s">
         <v>721</v>
@@ -21222,7 +21225,7 @@
         <v>723</v>
       </c>
       <c r="F68" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G68" s="120" t="s">
         <v>725</v>
@@ -21237,12 +21240,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B69" s="123" t="s">
-        <v>720</v>
+      <c r="B69" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C69" s="39" t="s">
         <v>721</v>
@@ -21253,8 +21256,8 @@
       <c r="E69" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F69" s="6" t="s">
-        <v>724</v>
+      <c r="F69" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G69" s="120" t="s">
         <v>725</v>
@@ -21269,12 +21272,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="28" t="s">
         <v>115</v>
       </c>
       <c r="B70" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C70" s="93" t="s">
         <v>721</v>
@@ -21286,7 +21289,7 @@
         <v>723</v>
       </c>
       <c r="F70" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G70" s="120" t="s">
         <v>725</v>
@@ -21301,12 +21304,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B71" s="123" t="s">
-        <v>720</v>
+      <c r="B71" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C71" s="39" t="s">
         <v>721</v>
@@ -21317,8 +21320,8 @@
       <c r="E71" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F71" s="6" t="s">
-        <v>724</v>
+      <c r="F71" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G71" s="120" t="s">
         <v>725</v>
@@ -21333,12 +21336,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="28" t="s">
         <v>119</v>
       </c>
       <c r="B72" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C72" s="93" t="s">
         <v>721</v>
@@ -21350,7 +21353,7 @@
         <v>723</v>
       </c>
       <c r="F72" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G72" s="120" t="s">
         <v>725</v>
@@ -21365,12 +21368,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="B73" s="123" t="s">
-        <v>720</v>
+      <c r="B73" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C73" s="39" t="s">
         <v>721</v>
@@ -21381,8 +21384,8 @@
       <c r="E73" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F73" s="6" t="s">
-        <v>724</v>
+      <c r="F73" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G73" s="120" t="s">
         <v>725</v>
@@ -21397,12 +21400,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="28" t="s">
         <v>123</v>
       </c>
       <c r="B74" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C74" s="93" t="s">
         <v>721</v>
@@ -21414,7 +21417,7 @@
         <v>723</v>
       </c>
       <c r="F74" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G74" s="120" t="s">
         <v>725</v>
@@ -21429,11 +21432,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="B75" s="123" t="s">
+      <c r="B75" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C75" s="39" t="s">
@@ -21445,8 +21448,8 @@
       <c r="E75" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F75" s="6" t="s">
-        <v>724</v>
+      <c r="F75" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G75" s="120" t="s">
         <v>725</v>
@@ -21461,7 +21464,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="28" t="s">
         <v>127</v>
       </c>
@@ -21478,7 +21481,7 @@
         <v>723</v>
       </c>
       <c r="F76" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G76" s="120" t="s">
         <v>725</v>
@@ -21493,11 +21496,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="B77" s="123" t="s">
+      <c r="B77" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C77" s="39" t="s">
@@ -21509,8 +21512,8 @@
       <c r="E77" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F77" s="6" t="s">
-        <v>724</v>
+      <c r="F77" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G77" s="120" t="s">
         <v>725</v>
@@ -21525,11 +21528,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="B78" s="125" t="s">
+      <c r="B78" s="123" t="s">
         <v>728</v>
       </c>
       <c r="C78" s="93" t="s">
@@ -21542,7 +21545,7 @@
         <v>723</v>
       </c>
       <c r="F78" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G78" s="120" t="s">
         <v>725</v>
@@ -21557,12 +21560,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="B79" s="119" t="s">
-        <v>720</v>
+      <c r="B79" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C79" s="39" t="s">
         <v>721</v>
@@ -21573,8 +21576,8 @@
       <c r="E79" s="121" t="s">
         <v>723</v>
       </c>
-      <c r="F79" s="6" t="s">
-        <v>724</v>
+      <c r="F79" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G79" s="120" t="s">
         <v>725</v>
@@ -21589,12 +21592,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="39" t="s">
         <v>135</v>
       </c>
       <c r="B80" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C80" s="93" t="s">
         <v>721</v>
@@ -21606,7 +21609,7 @@
         <v>723</v>
       </c>
       <c r="F80" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G80" s="120" t="s">
         <v>725</v>
@@ -21621,12 +21624,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="B81" s="123" t="s">
-        <v>720</v>
+      <c r="B81" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C81" s="39" t="s">
         <v>721</v>
@@ -21637,8 +21640,8 @@
       <c r="E81" s="17" t="s">
         <v>723</v>
       </c>
-      <c r="F81" s="6" t="s">
-        <v>724</v>
+      <c r="F81" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G81" s="120" t="s">
         <v>725</v>
@@ -21653,12 +21656,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="39" t="s">
         <v>139</v>
       </c>
       <c r="B82" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C82" s="93" t="s">
         <v>721</v>
@@ -21670,7 +21673,7 @@
         <v>723</v>
       </c>
       <c r="F82" s="65" t="s">
-        <v>724</v>
+        <v>1238</v>
       </c>
       <c r="G82" s="120" t="s">
         <v>725</v>
@@ -21685,12 +21688,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="B83" s="128" t="s">
-        <v>720</v>
+      <c r="B83" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C83" s="39" t="s">
         <v>721</v>
@@ -21701,8 +21704,8 @@
       <c r="E83" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F83" s="6" t="s">
-        <v>724</v>
+      <c r="F83" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G83" s="129" t="s">
         <v>725</v>
@@ -21717,12 +21720,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="B84" s="128" t="s">
-        <v>720</v>
+      <c r="B84" s="123" t="s">
+        <v>728</v>
       </c>
       <c r="C84" s="39" t="s">
         <v>721</v>
@@ -21733,8 +21736,8 @@
       <c r="E84" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F84" s="6" t="s">
-        <v>724</v>
+      <c r="F84" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G84" s="129" t="s">
         <v>725</v>
@@ -21749,12 +21752,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="35" t="s">
         <v>145</v>
       </c>
       <c r="B85" s="125" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C85" s="39" t="s">
         <v>721</v>
@@ -21765,8 +21768,8 @@
       <c r="E85" s="126" t="s">
         <v>723</v>
       </c>
-      <c r="F85" s="6" t="s">
-        <v>724</v>
+      <c r="F85" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G85" s="120" t="s">
         <v>725</v>
@@ -21781,12 +21784,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="B86" s="119" t="s">
-        <v>720</v>
+      <c r="B86" s="123" t="s">
+        <v>728</v>
       </c>
       <c r="C86" s="35" t="s">
         <v>721</v>
@@ -21813,12 +21816,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>767</v>
       </c>
-      <c r="B87" s="123" t="s">
-        <v>720</v>
+      <c r="B87" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C87" s="39" t="s">
         <v>721</v>
@@ -21845,12 +21848,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>768</v>
       </c>
       <c r="B88" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C88" s="93" t="s">
         <v>721</v>
@@ -21877,12 +21880,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
         <v>769</v>
       </c>
-      <c r="B89" s="123" t="s">
-        <v>720</v>
+      <c r="B89" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C89" s="39" t="s">
         <v>721</v>
@@ -21909,12 +21912,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
         <v>770</v>
       </c>
       <c r="B90" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C90" s="93" t="s">
         <v>721</v>
@@ -21941,12 +21944,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
         <v>771</v>
       </c>
-      <c r="B91" s="123" t="s">
-        <v>720</v>
+      <c r="B91" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C91" s="39" t="s">
         <v>721</v>
@@ -21973,12 +21976,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
         <v>772</v>
       </c>
       <c r="B92" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C92" s="93" t="s">
         <v>721</v>
@@ -22005,11 +22008,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
         <v>773</v>
       </c>
-      <c r="B93" s="123" t="s">
+      <c r="B93" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C93" s="39" t="s">
@@ -22037,7 +22040,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
         <v>774</v>
       </c>
@@ -22069,11 +22072,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>775</v>
       </c>
-      <c r="B95" s="123" t="s">
+      <c r="B95" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C95" s="39" t="s">
@@ -22101,7 +22104,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>776</v>
       </c>
@@ -22133,7 +22136,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="10" t="s">
         <v>777</v>
       </c>
@@ -22165,12 +22168,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="B98" s="119" t="s">
-        <v>720</v>
+      <c r="B98" s="123" t="s">
+        <v>728</v>
       </c>
       <c r="C98" s="93" t="s">
         <v>721</v>
@@ -22197,12 +22200,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B99" s="123" t="s">
-        <v>720</v>
+      <c r="B99" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C99" s="39" t="s">
         <v>721</v>
@@ -22229,12 +22232,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="17" t="s">
         <v>163</v>
       </c>
       <c r="B100" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C100" s="93" t="s">
         <v>721</v>
@@ -22261,12 +22264,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B101" s="123" t="s">
-        <v>720</v>
+      <c r="B101" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C101" s="39" t="s">
         <v>721</v>
@@ -22293,12 +22296,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="17" t="s">
         <v>167</v>
       </c>
       <c r="B102" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C102" s="93" t="s">
         <v>721</v>
@@ -22325,12 +22328,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="B103" s="123" t="s">
-        <v>720</v>
+      <c r="B103" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C103" s="39" t="s">
         <v>721</v>
@@ -22357,12 +22360,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="17" t="s">
         <v>171</v>
       </c>
       <c r="B104" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C104" s="93" t="s">
         <v>721</v>
@@ -22389,11 +22392,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="B105" s="123" t="s">
+      <c r="B105" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C105" s="39" t="s">
@@ -22421,7 +22424,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="17" t="s">
         <v>175</v>
       </c>
@@ -22453,11 +22456,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="B107" s="123" t="s">
+      <c r="B107" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C107" s="39" t="s">
@@ -22485,7 +22488,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="17" t="s">
         <v>179</v>
       </c>
@@ -22517,7 +22520,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="21" t="s">
         <v>181</v>
       </c>
@@ -22549,12 +22552,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="B110" s="119" t="s">
-        <v>720</v>
+      <c r="B110" s="123" t="s">
+        <v>728</v>
       </c>
       <c r="C110" s="93" t="s">
         <v>721</v>
@@ -22581,12 +22584,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="B111" s="123" t="s">
-        <v>720</v>
+      <c r="B111" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C111" s="39" t="s">
         <v>721</v>
@@ -22613,12 +22616,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="28" t="s">
         <v>187</v>
       </c>
       <c r="B112" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C112" s="93" t="s">
         <v>721</v>
@@ -22645,12 +22648,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="B113" s="123" t="s">
-        <v>720</v>
+      <c r="B113" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C113" s="39" t="s">
         <v>721</v>
@@ -22677,12 +22680,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="28" t="s">
         <v>191</v>
       </c>
       <c r="B114" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C114" s="93" t="s">
         <v>721</v>
@@ -22709,12 +22712,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="B115" s="123" t="s">
-        <v>720</v>
+      <c r="B115" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C115" s="39" t="s">
         <v>721</v>
@@ -22741,12 +22744,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="28" t="s">
         <v>195</v>
       </c>
       <c r="B116" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C116" s="93" t="s">
         <v>721</v>
@@ -22773,11 +22776,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="B117" s="123" t="s">
+      <c r="B117" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C117" s="39" t="s">
@@ -22805,7 +22808,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="28" t="s">
         <v>199</v>
       </c>
@@ -22837,11 +22840,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="B119" s="123" t="s">
+      <c r="B119" s="125" t="s">
         <v>728</v>
       </c>
       <c r="C119" s="39" t="s">
@@ -22869,11 +22872,11 @@
         <v>727</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="B120" s="125" t="s">
+      <c r="B120" s="123" t="s">
         <v>728</v>
       </c>
       <c r="C120" s="93" t="s">
@@ -22901,12 +22904,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="B121" s="119" t="s">
-        <v>720</v>
+      <c r="B121" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C121" s="39" t="s">
         <v>721</v>
@@ -22933,12 +22936,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="39" t="s">
         <v>207</v>
       </c>
       <c r="B122" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C122" s="93" t="s">
         <v>721</v>
@@ -22965,12 +22968,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="B123" s="123" t="s">
-        <v>720</v>
+      <c r="B123" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C123" s="39" t="s">
         <v>721</v>
@@ -22997,12 +23000,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="39" t="s">
         <v>211</v>
       </c>
       <c r="B124" s="123" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C124" s="93" t="s">
         <v>721</v>
@@ -23029,12 +23032,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="B125" s="128" t="s">
-        <v>720</v>
+      <c r="B125" s="125" t="s">
+        <v>728</v>
       </c>
       <c r="C125" s="39" t="s">
         <v>721</v>
@@ -23061,12 +23064,12 @@
         <v>727</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="39" t="s">
         <v>215</v>
       </c>
-      <c r="B126" s="128" t="s">
-        <v>720</v>
+      <c r="B126" s="123" t="s">
+        <v>728</v>
       </c>
       <c r="C126" s="39" t="s">
         <v>721</v>
@@ -23098,7 +23101,7 @@
         <v>217</v>
       </c>
       <c r="B127" s="125" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="C127" s="39" t="s">
         <v>721</v>
@@ -23130,7 +23133,7 @@
         <v>1112</v>
       </c>
       <c r="B128" s="152" t="s">
-        <v>1117</v>
+        <v>720</v>
       </c>
       <c r="C128" s="39" t="s">
         <v>721</v>
@@ -23141,8 +23144,8 @@
       <c r="E128" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F128" s="6" t="s">
-        <v>724</v>
+      <c r="F128" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G128" s="129" t="s">
         <v>725</v>
@@ -23162,7 +23165,7 @@
         <v>1113</v>
       </c>
       <c r="B129" s="152" t="s">
-        <v>1118</v>
+        <v>720</v>
       </c>
       <c r="C129" s="39" t="s">
         <v>721</v>
@@ -23173,8 +23176,8 @@
       <c r="E129" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F129" s="6" t="s">
-        <v>724</v>
+      <c r="F129" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G129" s="129" t="s">
         <v>725</v>
@@ -23194,7 +23197,7 @@
         <v>1114</v>
       </c>
       <c r="B130" s="152" t="s">
-        <v>1119</v>
+        <v>720</v>
       </c>
       <c r="C130" s="39" t="s">
         <v>721</v>
@@ -23205,8 +23208,8 @@
       <c r="E130" s="126" t="s">
         <v>723</v>
       </c>
-      <c r="F130" s="6" t="s">
-        <v>724</v>
+      <c r="F130" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G130" s="120" t="s">
         <v>725</v>
@@ -23226,7 +23229,7 @@
         <v>1115</v>
       </c>
       <c r="B131" s="152" t="s">
-        <v>1122</v>
+        <v>720</v>
       </c>
       <c r="C131" s="39" t="s">
         <v>721</v>
@@ -23237,8 +23240,8 @@
       <c r="E131" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F131" s="6" t="s">
-        <v>724</v>
+      <c r="F131" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G131" s="129" t="s">
         <v>725</v>
@@ -23258,7 +23261,7 @@
         <v>1116</v>
       </c>
       <c r="B132" s="152" t="s">
-        <v>1123</v>
+        <v>720</v>
       </c>
       <c r="C132" s="39" t="s">
         <v>721</v>
@@ -23269,8 +23272,8 @@
       <c r="E132" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F132" s="6" t="s">
-        <v>724</v>
+      <c r="F132" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G132" s="129" t="s">
         <v>725</v>
@@ -23290,7 +23293,7 @@
         <v>1121</v>
       </c>
       <c r="B133" s="152" t="s">
-        <v>1125</v>
+        <v>720</v>
       </c>
       <c r="C133" s="39" t="s">
         <v>721</v>
@@ -23301,8 +23304,8 @@
       <c r="E133" s="126" t="s">
         <v>723</v>
       </c>
-      <c r="F133" s="6" t="s">
-        <v>724</v>
+      <c r="F133" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G133" s="120" t="s">
         <v>725</v>
@@ -23322,7 +23325,7 @@
         <v>1120</v>
       </c>
       <c r="B134" s="152" t="s">
-        <v>1126</v>
+        <v>720</v>
       </c>
       <c r="C134" s="39" t="s">
         <v>721</v>
@@ -23333,8 +23336,8 @@
       <c r="E134" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F134" s="6" t="s">
-        <v>724</v>
+      <c r="F134" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G134" s="129" t="s">
         <v>725</v>
@@ -23353,8 +23356,8 @@
       <c r="A135" s="155" t="s">
         <v>1127</v>
       </c>
-      <c r="B135" s="156" t="s">
-        <v>1134</v>
+      <c r="B135" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C135" s="39" t="s">
         <v>721</v>
@@ -23365,8 +23368,8 @@
       <c r="E135" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F135" s="6" t="s">
-        <v>724</v>
+      <c r="F135" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G135" s="129" t="s">
         <v>725</v>
@@ -23385,8 +23388,8 @@
       <c r="A136" s="155" t="s">
         <v>1128</v>
       </c>
-      <c r="B136" s="156" t="s">
-        <v>1135</v>
+      <c r="B136" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C136" s="39" t="s">
         <v>721</v>
@@ -23397,8 +23400,8 @@
       <c r="E136" s="126" t="s">
         <v>723</v>
       </c>
-      <c r="F136" s="6" t="s">
-        <v>724</v>
+      <c r="F136" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G136" s="120" t="s">
         <v>725</v>
@@ -23417,8 +23420,8 @@
       <c r="A137" s="155" t="s">
         <v>1129</v>
       </c>
-      <c r="B137" s="156" t="s">
-        <v>1136</v>
+      <c r="B137" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C137" s="39" t="s">
         <v>721</v>
@@ -23429,8 +23432,8 @@
       <c r="E137" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F137" s="6" t="s">
-        <v>724</v>
+      <c r="F137" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G137" s="129" t="s">
         <v>725</v>
@@ -23449,8 +23452,8 @@
       <c r="A138" s="155" t="s">
         <v>1130</v>
       </c>
-      <c r="B138" s="156" t="s">
-        <v>1137</v>
+      <c r="B138" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C138" s="39" t="s">
         <v>721</v>
@@ -23461,8 +23464,8 @@
       <c r="E138" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F138" s="6" t="s">
-        <v>724</v>
+      <c r="F138" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G138" s="129" t="s">
         <v>725</v>
@@ -23481,8 +23484,8 @@
       <c r="A139" s="155" t="s">
         <v>1131</v>
       </c>
-      <c r="B139" s="156" t="s">
-        <v>1138</v>
+      <c r="B139" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C139" s="39" t="s">
         <v>721</v>
@@ -23493,8 +23496,8 @@
       <c r="E139" s="126" t="s">
         <v>723</v>
       </c>
-      <c r="F139" s="6" t="s">
-        <v>724</v>
+      <c r="F139" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G139" s="120" t="s">
         <v>725</v>
@@ -23513,8 +23516,8 @@
       <c r="A140" s="155" t="s">
         <v>1132</v>
       </c>
-      <c r="B140" s="156" t="s">
-        <v>1139</v>
+      <c r="B140" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C140" s="39" t="s">
         <v>721</v>
@@ -23525,8 +23528,8 @@
       <c r="E140" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F140" s="6" t="s">
-        <v>724</v>
+      <c r="F140" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G140" s="129" t="s">
         <v>725</v>
@@ -23545,8 +23548,8 @@
       <c r="A141" s="155" t="s">
         <v>1133</v>
       </c>
-      <c r="B141" s="156" t="s">
-        <v>1140</v>
+      <c r="B141" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C141" s="39" t="s">
         <v>721</v>
@@ -23557,8 +23560,8 @@
       <c r="E141" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F141" s="6" t="s">
-        <v>724</v>
+      <c r="F141" s="65" t="s">
+        <v>1238</v>
       </c>
       <c r="G141" s="129" t="s">
         <v>725</v>
@@ -23577,8 +23580,8 @@
       <c r="A142" s="39" t="s">
         <v>1141</v>
       </c>
-      <c r="B142" s="148" t="s">
-        <v>1148</v>
+      <c r="B142" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C142" s="39" t="s">
         <v>721</v>
@@ -23589,7 +23592,7 @@
       <c r="E142" s="126" t="s">
         <v>723</v>
       </c>
-      <c r="F142" s="6" t="s">
+      <c r="F142" s="65" t="s">
         <v>724</v>
       </c>
       <c r="G142" s="120" t="s">
@@ -23609,8 +23612,8 @@
       <c r="A143" s="39" t="s">
         <v>1142</v>
       </c>
-      <c r="B143" s="148" t="s">
-        <v>1149</v>
+      <c r="B143" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C143" s="39" t="s">
         <v>721</v>
@@ -23621,7 +23624,7 @@
       <c r="E143" s="130" t="s">
         <v>723</v>
       </c>
-      <c r="F143" s="6" t="s">
+      <c r="F143" s="65" t="s">
         <v>724</v>
       </c>
       <c r="G143" s="129" t="s">
@@ -23641,8 +23644,8 @@
       <c r="A144" s="39" t="s">
         <v>1143</v>
       </c>
-      <c r="B144" s="148" t="s">
-        <v>1150</v>
+      <c r="B144" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C144" s="39" t="s">
         <v>721</v>
@@ -23673,8 +23676,8 @@
       <c r="A145" s="39" t="s">
         <v>1144</v>
       </c>
-      <c r="B145" s="148" t="s">
-        <v>1151</v>
+      <c r="B145" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C145" s="39" t="s">
         <v>721</v>
@@ -23705,8 +23708,8 @@
       <c r="A146" s="39" t="s">
         <v>1145</v>
       </c>
-      <c r="B146" s="148" t="s">
-        <v>1152</v>
+      <c r="B146" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C146" s="39" t="s">
         <v>721</v>
@@ -23737,8 +23740,8 @@
       <c r="A147" s="39" t="s">
         <v>1146</v>
       </c>
-      <c r="B147" s="148" t="s">
-        <v>1124</v>
+      <c r="B147" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C147" s="39" t="s">
         <v>721</v>
@@ -23769,8 +23772,8 @@
       <c r="A148" s="39" t="s">
         <v>1147</v>
       </c>
-      <c r="B148" s="148" t="s">
-        <v>1153</v>
+      <c r="B148" s="152" t="s">
+        <v>728</v>
       </c>
       <c r="C148" s="39" t="s">
         <v>721</v>
@@ -28453,18 +28456,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28638,6 +28641,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -28649,14 +28660,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>